<commit_message>
start development + logboek
</commit_message>
<xml_diff>
--- a/documentatie/logboek/personlijke_logboek/logboek Santi Dudok.xlsx
+++ b/documentatie/logboek/personlijke_logboek/logboek Santi Dudok.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>bereikbaarheidslijst</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>het gaat tot nu toe goed</t>
+  </si>
+  <si>
+    <t>yields klaar</t>
+  </si>
+  <si>
+    <t>1 uur</t>
+  </si>
+  <si>
+    <t>was heel makkelijk</t>
+  </si>
+  <si>
+    <t>begonnen met development page</t>
   </si>
 </sst>
 </file>
@@ -547,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99C9DD8-8A8E-4C8E-A99F-612C0B641610}">
   <dimension ref="I7:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,16 +811,32 @@
       </c>
     </row>
     <row r="24" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="I24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K24" s="4">
+        <v>43020</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="25" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="26" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I26" s="3"/>

</xml_diff>

<commit_message>
Development front-end klaar + logboek
</commit_message>
<xml_diff>
--- a/documentatie/logboek/personlijke_logboek/logboek Santi Dudok.xlsx
+++ b/documentatie/logboek/personlijke_logboek/logboek Santi Dudok.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>bereikbaarheidslijst</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>begonnen met development page</t>
+  </si>
+  <si>
+    <t>development front-end af</t>
+  </si>
+  <si>
+    <t>Het ging redelijk simpel op een paar bugs na</t>
   </si>
 </sst>
 </file>
@@ -237,12 +243,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -559,15 +567,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99C9DD8-8A8E-4C8E-A99F-612C0B641610}">
   <dimension ref="I7:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="8" width="8.88671875" style="2"/>
     <col min="9" max="9" width="16.88671875" style="2" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" style="2"/>
+    <col min="10" max="10" width="8.88671875" style="2"/>
+    <col min="11" max="11" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="57.109375" style="2" customWidth="1"/>
     <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -839,10 +848,18 @@
       </c>
     </row>
     <row r="26" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="I26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="6">
+        <v>43031</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="27" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I27" s="3"/>

</xml_diff>